<commit_message>
fixed excel files and extend report paths
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CurtA\SQA-Workspace\SQASeleniumProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF89B58-7ED9-4E9D-BD56-DE58AB708A0F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" xr2:uid="{D9A4D28E-4C18-457D-BDD1-3DE3F2ED2DC7}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -35,18 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>mngr119144</t>
-  </si>
-  <si>
-    <t>YjAqumY</t>
-  </si>
-  <si>
-    <t>mngr119484</t>
-  </si>
-  <si>
-    <t>gagumug</t>
-  </si>
-  <si>
     <t>TC_Valid1</t>
   </si>
   <si>
@@ -56,10 +45,10 @@
     <t>TC_Valid3</t>
   </si>
   <si>
-    <t>mngr119145</t>
-  </si>
-  <si>
-    <t>jErenYm</t>
+    <t>mngr122407</t>
+  </si>
+  <si>
+    <t>apYsUtA</t>
   </si>
 </sst>
 </file>
@@ -414,10 +403,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -432,35 +425,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added parasoft and properties
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CurtA\SQA-Workspace\SQASeleniumProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF89B58-7ED9-4E9D-BD56-DE58AB708A0F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0028402-393A-4DF3-B5E0-DB3C97A620D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" xr2:uid="{D9A4D28E-4C18-457D-BDD1-3DE3F2ED2DC7}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>TC_Valid3</t>
   </si>
   <si>
-    <t>mngr122407</t>
-  </si>
-  <si>
-    <t>apYsUtA</t>
+    <t>mngr126739</t>
+  </si>
+  <si>
+    <t>netyveb</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>